<commit_message>
Final version for Ardi and Randa
</commit_message>
<xml_diff>
--- a/iron_data/all_iron_data_corrected.xlsx
+++ b/iron_data/all_iron_data_corrected.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/PyCharm/IronUptake/iron_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A783CF92-BD1C-2340-92A9-7C34202111AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778B68D4-639F-D642-B31F-3E386DBF8D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="2" xr2:uid="{A78AB3EF-5C49-4870-8BEB-C0E596962EEB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{A78AB3EF-5C49-4870-8BEB-C0E596962EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Content and Concentration (1)" sheetId="1" r:id="rId1"/>
-    <sheet name="Iron_in_matrix" sheetId="2" r:id="rId2"/>
-    <sheet name="Iron_in_plants" sheetId="3" r:id="rId3"/>
+    <sheet name="Iron_dose" sheetId="4" r:id="rId2"/>
+    <sheet name="Iron_in_matrix" sheetId="2" r:id="rId3"/>
+    <sheet name="Iron_in_plants" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="540">
   <si>
     <t>concentration of iron</t>
   </si>
@@ -1711,7 +1712,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1739,12 +1740,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="207">
@@ -3555,17 +3550,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4557300B-D54B-4877-8D48-390F8C8345AC}">
   <dimension ref="A1:CL94"/>
   <sheetViews>
-    <sheetView topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CE2" sqref="CE2:CE61"/>
+    <sheetView topLeftCell="BV1" workbookViewId="0">
+      <selection activeCell="CH2" sqref="CH2:CH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="9" max="9" width="27.83203125" style="2" customWidth="1"/>
     <col min="10" max="12" width="20.5" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="20.33203125" customWidth="1"/>
@@ -3574,19 +3571,25 @@
     <col min="17" max="17" width="14.33203125" customWidth="1"/>
     <col min="18" max="18" width="17.33203125" customWidth="1"/>
     <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="19.5" customWidth="1"/>
     <col min="22" max="22" width="15.6640625" style="2" customWidth="1"/>
     <col min="23" max="25" width="15.6640625" style="3" customWidth="1"/>
     <col min="26" max="26" width="9.1640625" style="5"/>
     <col min="31" max="31" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="8.83203125" customWidth="1"/>
     <col min="35" max="35" width="13.83203125" style="2" customWidth="1"/>
     <col min="36" max="38" width="15.6640625" style="3" customWidth="1"/>
     <col min="39" max="39" width="9.1640625" style="5"/>
     <col min="44" max="44" width="19.5" customWidth="1"/>
+    <col min="47" max="47" width="18.6640625" customWidth="1"/>
     <col min="48" max="48" width="16.1640625" style="2" customWidth="1"/>
     <col min="49" max="51" width="15.6640625" style="3" customWidth="1"/>
     <col min="52" max="52" width="9.1640625" style="5"/>
     <col min="57" max="57" width="16.83203125" customWidth="1"/>
-    <col min="61" max="61" width="23" style="2" customWidth="1"/>
+    <col min="58" max="58" width="15.83203125" customWidth="1"/>
+    <col min="59" max="59" width="25.1640625" customWidth="1"/>
+    <col min="60" max="60" width="35" customWidth="1"/>
+    <col min="61" max="61" width="29.5" style="2" customWidth="1"/>
     <col min="62" max="64" width="15.6640625" style="3" customWidth="1"/>
     <col min="65" max="65" width="9.1640625" style="5"/>
     <col min="70" max="70" width="16.83203125" customWidth="1"/>
@@ -3594,7 +3597,7 @@
     <col min="75" max="77" width="15.6640625" style="3" customWidth="1"/>
     <col min="78" max="78" width="9.1640625" style="5"/>
     <col min="83" max="83" width="16.83203125" customWidth="1"/>
-    <col min="87" max="87" width="17.1640625" style="2" customWidth="1"/>
+    <col min="87" max="87" width="27.83203125" style="2" customWidth="1"/>
     <col min="88" max="90" width="15.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10157,7 +10160,7 @@
         <v>5.3852024498529202E-2</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="38"/>
+        <f>AF23+AF53</f>
         <v>0.11127928810458181</v>
       </c>
       <c r="AH23">
@@ -16918,17 +16921,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90849AF7-0A25-6F4C-8419-6629EAF8DF97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254E9761-C84A-CA42-A8EB-A0767C8AF6F9}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -16961,25 +16961,25 @@
         <v>510</v>
       </c>
       <c r="B2">
-        <v>0.71506606636420611</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="C2">
-        <v>0.71875414905100699</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="D2">
-        <v>0.71878960437917483</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="E2">
-        <v>0.73483872890988067</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="F2">
-        <v>0.69827372092176354</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="G2">
-        <v>0.71132210175877486</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="H2">
-        <v>0.71798852441300909</v>
+        <v>0.75390000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -16987,25 +16987,25 @@
         <v>511</v>
       </c>
       <c r="B3">
-        <v>0.71930850747545938</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="C3">
-        <v>0.73279883762855391</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="D3">
-        <v>0.71950895454363284</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="E3">
-        <v>0.67085233754564511</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="F3">
-        <v>0.712851149029882</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="G3">
-        <v>0.70943913644933754</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="H3">
-        <v>0.71792916718044419</v>
+        <v>0.75390000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -17013,25 +17013,25 @@
         <v>512</v>
       </c>
       <c r="B4">
-        <v>0.72042250966937482</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="C4">
-        <v>0.719676922381005</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="D4">
-        <v>0.68832570326084352</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="E4">
-        <v>0.72472727991406094</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="F4">
-        <v>0.7178411639629052</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="G4">
-        <v>0.72671226712123815</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="H4">
-        <v>0.72056820032356894</v>
+        <v>0.75390000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -17039,25 +17039,25 @@
         <v>513</v>
       </c>
       <c r="B5">
-        <v>0.7327841421442034</v>
+        <v>0.77065349999999999</v>
       </c>
       <c r="C5">
-        <v>0.75837353996422985</v>
+        <v>0.79578375000000001</v>
       </c>
       <c r="D5">
-        <v>0.78911121476067592</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="E5">
-        <v>0.80686308241646199</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="F5">
-        <v>0.84193549043933091</v>
+        <v>0.921435</v>
       </c>
       <c r="G5">
-        <v>0.96692063456835076</v>
+        <v>1.0052025</v>
       </c>
       <c r="H5">
-        <v>1.0508583090860291</v>
+        <v>1.08897</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -17065,25 +17065,25 @@
         <v>514</v>
       </c>
       <c r="B6">
-        <v>0.72886620848632955</v>
+        <v>0.77065349999999999</v>
       </c>
       <c r="C6">
-        <v>0.7629800309157897</v>
+        <v>0.79578375000000001</v>
       </c>
       <c r="D6">
-        <v>0.76619784691551795</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="E6">
-        <v>0.83160345541385594</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="F6">
-        <v>0.85258717907249248</v>
+        <v>0.921435</v>
       </c>
       <c r="G6">
-        <v>0.95308759093767237</v>
+        <v>1.0052025</v>
       </c>
       <c r="H6">
-        <v>1.0521606268629349</v>
+        <v>1.08897</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -17091,25 +17091,25 @@
         <v>515</v>
       </c>
       <c r="B7">
-        <v>0.73249387570363367</v>
+        <v>0.77065349999999999</v>
       </c>
       <c r="C7">
-        <v>0.77141559424394479</v>
+        <v>0.79578375000000001</v>
       </c>
       <c r="D7">
-        <v>0.78345633332101328</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="E7">
-        <v>0.82769712527798345</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="F7">
-        <v>0.87717409489236253</v>
+        <v>0.921435</v>
       </c>
       <c r="G7">
-        <v>0.93657512778600482</v>
+        <v>1.0052025</v>
       </c>
       <c r="H7">
-        <v>1.0460454927207554</v>
+        <v>1.08897</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -17117,25 +17117,25 @@
         <v>516</v>
       </c>
       <c r="B8">
-        <v>0.74545674082706359</v>
+        <v>0.78740699999999997</v>
       </c>
       <c r="C8">
-        <v>0.77640338673542553</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="D8">
-        <v>0.87554086006001952</v>
+        <v>0.921435</v>
       </c>
       <c r="E8">
-        <v>0.93002386042631613</v>
+        <v>1.0052025</v>
       </c>
       <c r="F8">
-        <v>1.0135770467467382</v>
+        <v>1.08897</v>
       </c>
       <c r="G8">
-        <v>1.1916271002672496</v>
+        <v>1.256505</v>
       </c>
       <c r="H8">
-        <v>1.3682058128223209</v>
+        <v>1.42404</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -17143,25 +17143,25 @@
         <v>517</v>
       </c>
       <c r="B9">
-        <v>0.73134484996061833</v>
+        <v>0.78740699999999997</v>
       </c>
       <c r="C9">
-        <v>0.78031584562080691</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="D9">
-        <v>0.85344274338729187</v>
+        <v>0.921435</v>
       </c>
       <c r="E9">
-        <v>0.9417001606580333</v>
+        <v>1.0052025</v>
       </c>
       <c r="F9">
-        <v>0.98029133960329295</v>
+        <v>1.08897</v>
       </c>
       <c r="G9">
-        <v>1.2184403249679672</v>
+        <v>1.256505</v>
       </c>
       <c r="H9">
-        <v>1.3883721120774239</v>
+        <v>1.42404</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -17169,25 +17169,25 @@
         <v>518</v>
       </c>
       <c r="B10">
-        <v>0.75368254108109334</v>
+        <v>0.78740699999999997</v>
       </c>
       <c r="C10">
-        <v>0.79063935881460834</v>
+        <v>0.83766750000000001</v>
       </c>
       <c r="D10">
-        <v>0.85136128949685708</v>
+        <v>0.921435</v>
       </c>
       <c r="E10">
-        <v>0.95365599832833148</v>
+        <v>1.0052025</v>
       </c>
       <c r="F10">
-        <v>1.003892438666705</v>
+        <v>1.08897</v>
       </c>
       <c r="G10">
-        <v>1.2108544348995876</v>
+        <v>1.256505</v>
       </c>
       <c r="H10">
-        <v>1.3669423981284534</v>
+        <v>1.42404</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -17195,25 +17195,25 @@
         <v>519</v>
       </c>
       <c r="B11">
-        <v>0.74151365059006102</v>
+        <v>0.80416049999999994</v>
       </c>
       <c r="C11">
-        <v>0.78779187774599635</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="D11">
-        <v>0.93318519185444504</v>
+        <v>1.0052025</v>
       </c>
       <c r="E11">
-        <v>0.99544307791096376</v>
+        <v>1.13085375</v>
       </c>
       <c r="F11">
-        <v>1.1515747878657849</v>
+        <v>1.256505</v>
       </c>
       <c r="G11">
-        <v>1.3798851081578447</v>
+        <v>1.5078075</v>
       </c>
       <c r="H11">
-        <v>1.6233293932464679</v>
+        <v>1.75911</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -17221,25 +17221,25 @@
         <v>520</v>
       </c>
       <c r="B12">
-        <v>0.74648738640105383</v>
+        <v>0.80416049999999994</v>
       </c>
       <c r="C12">
-        <v>0.80061919820982685</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="D12">
-        <v>0.9228335443639154</v>
+        <v>1.0052025</v>
       </c>
       <c r="E12">
-        <v>1.0489739085129681</v>
+        <v>1.13085375</v>
       </c>
       <c r="F12">
-        <v>1.1764015544272659</v>
+        <v>1.256505</v>
       </c>
       <c r="G12">
-        <v>1.4179965114028932</v>
+        <v>1.5078075</v>
       </c>
       <c r="H12">
-        <v>1.6201968720808102</v>
+        <v>1.75911</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -17247,25 +17247,25 @@
         <v>521</v>
       </c>
       <c r="B13">
-        <v>0.71791545827826397</v>
+        <v>0.80416049999999994</v>
       </c>
       <c r="C13">
-        <v>0.78415922648608216</v>
+        <v>0.87955125000000001</v>
       </c>
       <c r="D13">
-        <v>0.93463851901856287</v>
+        <v>1.0052025</v>
       </c>
       <c r="E13">
-        <v>0.97484918920504005</v>
+        <v>1.13085375</v>
       </c>
       <c r="F13">
-        <v>1.1376103785813734</v>
+        <v>1.256505</v>
       </c>
       <c r="G13">
-        <v>1.409869777328929</v>
+        <v>1.5078075</v>
       </c>
       <c r="H13">
-        <v>1.6804032634972041</v>
+        <v>1.75911</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -17273,25 +17273,25 @@
         <v>522</v>
       </c>
       <c r="B14">
-        <v>0.74816875014755269</v>
+        <v>0.82091399999999992</v>
       </c>
       <c r="C14">
-        <v>0.86000179250885522</v>
+        <v>0.921435</v>
       </c>
       <c r="D14">
-        <v>0.99202876321940248</v>
+        <v>1.08897</v>
       </c>
       <c r="E14">
-        <v>1.106882524666176</v>
+        <v>1.256505</v>
       </c>
       <c r="F14">
-        <v>1.271525229991975</v>
+        <v>1.42404</v>
       </c>
       <c r="G14">
-        <v>1.6630012092858513</v>
+        <v>1.75911</v>
       </c>
       <c r="H14">
-        <v>1.9739084516002943</v>
+        <v>2.0941799999999997</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17299,25 +17299,25 @@
         <v>523</v>
       </c>
       <c r="B15">
-        <v>0.74402770838118248</v>
+        <v>0.82091399999999992</v>
       </c>
       <c r="C15">
-        <v>0.83323127956731713</v>
+        <v>0.921435</v>
       </c>
       <c r="D15">
-        <v>0.99030454057501482</v>
+        <v>1.08897</v>
       </c>
       <c r="E15">
-        <v>1.148105671475143</v>
+        <v>1.256505</v>
       </c>
       <c r="F15">
-        <v>1.2924488355750139</v>
+        <v>1.42404</v>
       </c>
       <c r="G15">
-        <v>1.6286030365182178</v>
+        <v>1.75911</v>
       </c>
       <c r="H15">
-        <v>1.9626391788486983</v>
+        <v>2.0941799999999997</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -17325,25 +17325,25 @@
         <v>524</v>
       </c>
       <c r="B16">
-        <v>0.76045102045789126</v>
+        <v>0.82091399999999992</v>
       </c>
       <c r="C16">
-        <v>0.80575934294169627</v>
+        <v>0.921435</v>
       </c>
       <c r="D16">
-        <v>0.99772746424023706</v>
+        <v>1.08897</v>
       </c>
       <c r="E16">
-        <v>1.1136598290172319</v>
+        <v>1.256505</v>
       </c>
       <c r="F16">
-        <v>1.3097505496432953</v>
+        <v>1.42404</v>
       </c>
       <c r="G16">
-        <v>1.6368500540303836</v>
+        <v>1.75911</v>
       </c>
       <c r="H16">
-        <v>1.9342212348138714</v>
+        <v>2.0941799999999997</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -17351,25 +17351,25 @@
         <v>525</v>
       </c>
       <c r="B17">
-        <v>0.75932316397975175</v>
+        <v>0.8376674999999999</v>
       </c>
       <c r="C17">
-        <v>0.85654125388649405</v>
+        <v>0.96331875</v>
       </c>
       <c r="D17">
-        <v>1.0940566366973026</v>
+        <v>1.1727375</v>
       </c>
       <c r="E17">
-        <v>1.2641572562408654</v>
+        <v>1.38215625</v>
       </c>
       <c r="F17">
-        <v>1.3603507568514812</v>
+        <v>1.591575</v>
       </c>
       <c r="G17">
-        <v>1.8682597554883291</v>
+        <v>2.0104125000000002</v>
       </c>
       <c r="H17">
-        <v>2.265565520560977</v>
+        <v>2.4292499999999997</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -17377,25 +17377,25 @@
         <v>526</v>
       </c>
       <c r="B18">
-        <v>0.76394055505756375</v>
+        <v>0.8376674999999999</v>
       </c>
       <c r="C18">
-        <v>0.83955447625866475</v>
+        <v>0.96331875</v>
       </c>
       <c r="D18">
-        <v>1.077739119764803</v>
+        <v>1.1727375</v>
       </c>
       <c r="E18">
-        <v>1.2473540671058958</v>
+        <v>1.38215625</v>
       </c>
       <c r="F18">
-        <v>1.4268471575976192</v>
+        <v>1.591575</v>
       </c>
       <c r="G18">
-        <v>1.8301032203667333</v>
+        <v>2.0104125000000002</v>
       </c>
       <c r="H18">
-        <v>2.2374402954195487</v>
+        <v>2.4292499999999997</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -17403,25 +17403,25 @@
         <v>527</v>
       </c>
       <c r="B19">
-        <v>0.76859639269493063</v>
+        <v>0.8376674999999999</v>
       </c>
       <c r="C19">
-        <v>0.87373962763963708</v>
+        <v>0.96331875</v>
       </c>
       <c r="D19">
-        <v>1.0904070640626575</v>
+        <v>1.1727375</v>
       </c>
       <c r="E19">
-        <v>1.3009046599959579</v>
+        <v>1.38215625</v>
       </c>
       <c r="F19">
-        <v>1.3678700570538189</v>
+        <v>1.591575</v>
       </c>
       <c r="G19">
-        <v>1.8857335756450007</v>
+        <v>2.0104125000000002</v>
       </c>
       <c r="H19">
-        <v>2.3209693131335309</v>
+        <v>2.4292499999999997</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -17429,25 +17429,25 @@
         <v>528</v>
       </c>
       <c r="B20">
-        <v>0.75076441276244199</v>
+        <v>0.85442099999999988</v>
       </c>
       <c r="C20">
-        <v>0.89181819830966214</v>
+        <v>1.0052025</v>
       </c>
       <c r="D20">
-        <v>1.0920465333961462</v>
+        <v>1.256505</v>
       </c>
       <c r="E20">
-        <v>1.3549203941106067</v>
+        <v>1.5078075</v>
       </c>
       <c r="F20">
-        <v>1.5703040395546182</v>
+        <v>1.75911</v>
       </c>
       <c r="G20">
-        <v>2.01710612030806</v>
+        <v>2.2617150000000001</v>
       </c>
       <c r="H20">
-        <v>2.5935679372091425</v>
+        <v>2.7643199999999997</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -17455,25 +17455,25 @@
         <v>529</v>
       </c>
       <c r="B21">
-        <v>0.75215206942020041</v>
+        <v>0.85442099999999988</v>
       </c>
       <c r="C21">
-        <v>0.91154060063879161</v>
+        <v>1.0052025</v>
       </c>
       <c r="D21">
-        <v>1.1311640039954942</v>
+        <v>1.256505</v>
       </c>
       <c r="E21">
-        <v>1.3825586413549611</v>
+        <v>1.5078075</v>
       </c>
       <c r="F21">
-        <v>1.5084480781979113</v>
+        <v>1.75911</v>
       </c>
       <c r="G21">
-        <v>1.995170113813534</v>
+        <v>2.2617150000000001</v>
       </c>
       <c r="H21">
-        <v>2.5531692765459795</v>
+        <v>2.7643199999999997</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -17481,25 +17481,25 @@
         <v>530</v>
       </c>
       <c r="B22">
-        <v>0.75075202637915883</v>
+        <v>0.85442099999999988</v>
       </c>
       <c r="C22">
-        <v>0.89195921474632678</v>
+        <v>1.0052025</v>
       </c>
       <c r="D22">
-        <v>1.0701021754728139</v>
+        <v>1.256505</v>
       </c>
       <c r="E22">
-        <v>1.2947901572792393</v>
+        <v>1.5078075</v>
       </c>
       <c r="F22">
-        <v>1.5825791590737568</v>
+        <v>1.75911</v>
       </c>
       <c r="G22">
-        <v>2.0669666029486358</v>
+        <v>2.2617150000000001</v>
       </c>
       <c r="H22">
-        <v>2.5658833659827831</v>
+        <v>2.7643199999999997</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -17507,25 +17507,25 @@
         <v>531</v>
       </c>
       <c r="B23">
-        <v>0.77808854720814047</v>
+        <v>0.87117449999999985</v>
       </c>
       <c r="C23">
-        <v>0.97339231188897368</v>
+        <v>1.04708625</v>
       </c>
       <c r="D23">
-        <v>1.2289932118954181</v>
+        <v>1.3402725</v>
       </c>
       <c r="E23">
-        <v>1.4550010801515059</v>
+        <v>1.63345875</v>
       </c>
       <c r="F23">
-        <v>1.6462933853711921</v>
+        <v>1.9266449999999999</v>
       </c>
       <c r="G23">
-        <v>2.268265054363432</v>
+        <v>2.5130175000000001</v>
       </c>
       <c r="H23">
-        <v>2.8531738815834191</v>
+        <v>3.0993899999999996</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -17533,25 +17533,25 @@
         <v>532</v>
       </c>
       <c r="B24">
-        <v>0.75011504251102457</v>
+        <v>0.87117449999999985</v>
       </c>
       <c r="C24">
-        <v>0.92391775522547703</v>
+        <v>1.04708625</v>
       </c>
       <c r="D24">
-        <v>1.1576837107999587</v>
+        <v>1.3402725</v>
       </c>
       <c r="E24">
-        <v>1.4384355818112371</v>
+        <v>1.63345875</v>
       </c>
       <c r="F24">
-        <v>1.6510457401620728</v>
+        <v>1.9266449999999999</v>
       </c>
       <c r="G24">
-        <v>2.2713150393919093</v>
+        <v>2.5130175000000001</v>
       </c>
       <c r="H24">
-        <v>2.8608978694063394</v>
+        <v>3.0993899999999996</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -17559,25 +17559,25 @@
         <v>533</v>
       </c>
       <c r="B25">
-        <v>0.76566754043071117</v>
+        <v>0.87117449999999985</v>
       </c>
       <c r="C25">
-        <v>0.92281376485356748</v>
+        <v>1.04708625</v>
       </c>
       <c r="D25">
-        <v>1.2136617596610122</v>
+        <v>1.3402725</v>
       </c>
       <c r="E25">
-        <v>1.4091527486942568</v>
+        <v>1.63345875</v>
       </c>
       <c r="F25">
-        <v>1.6199667056041895</v>
+        <v>1.9266449999999999</v>
       </c>
       <c r="G25">
-        <v>2.3223452272518079</v>
+        <v>2.5130175000000001</v>
       </c>
       <c r="H25">
-        <v>2.7962117981393888</v>
+        <v>3.0993899999999996</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -17585,25 +17585,25 @@
         <v>534</v>
       </c>
       <c r="B26">
-        <v>0.71100664638581534</v>
+        <v>0.88792799999999983</v>
       </c>
       <c r="C26">
-        <v>1.0160446101234422</v>
+        <v>1.08897</v>
       </c>
       <c r="D26">
-        <v>1.2223302609742199</v>
+        <v>1.42404</v>
       </c>
       <c r="E26">
-        <v>1.5737299995929364</v>
+        <v>1.75911</v>
       </c>
       <c r="F26">
-        <v>1.8140642925867696</v>
+        <v>2.0941799999999997</v>
       </c>
       <c r="G26">
-        <v>2.4965088734340215</v>
+        <v>2.7643200000000001</v>
       </c>
       <c r="H26">
-        <v>3.1705133391543554</v>
+        <v>3.4344599999999996</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -17611,25 +17611,25 @@
         <v>535</v>
       </c>
       <c r="B27">
-        <v>0.772714033380697</v>
+        <v>0.88792799999999983</v>
       </c>
       <c r="C27">
-        <v>0.8926641220591025</v>
+        <v>1.08897</v>
       </c>
       <c r="D27">
-        <v>1.2223601351633306</v>
+        <v>1.42404</v>
       </c>
       <c r="E27">
-        <v>1.5389342867585005</v>
+        <v>1.75911</v>
       </c>
       <c r="F27">
-        <v>1.7969707715812695</v>
+        <v>2.0941799999999997</v>
       </c>
       <c r="G27">
-        <v>2.5207792896816907</v>
+        <v>2.7643200000000001</v>
       </c>
       <c r="H27">
-        <v>3.2370190613221776</v>
+        <v>3.4344599999999996</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -17637,25 +17637,25 @@
         <v>536</v>
       </c>
       <c r="B28">
-        <v>0.77669151330420372</v>
+        <v>0.88792799999999983</v>
       </c>
       <c r="C28">
-        <v>0.94544055628202328</v>
+        <v>1.08897</v>
       </c>
       <c r="D28">
-        <v>1.2976233116485889</v>
+        <v>1.42404</v>
       </c>
       <c r="E28">
-        <v>1.5756365434182478</v>
+        <v>1.75911</v>
       </c>
       <c r="F28">
-        <v>1.8075258575785609</v>
+        <v>2.0941799999999997</v>
       </c>
       <c r="G28">
-        <v>2.4602937099866953</v>
+        <v>2.7643200000000001</v>
       </c>
       <c r="H28">
-        <v>3.1584168705730828</v>
+        <v>3.4344599999999996</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -17663,25 +17663,25 @@
         <v>537</v>
       </c>
       <c r="B29">
-        <v>0.7804707471730471</v>
+        <v>0.90468149999999981</v>
       </c>
       <c r="C29">
-        <v>0.9776623785413846</v>
+        <v>1.13085375</v>
       </c>
       <c r="D29">
-        <v>1.3761953177319712</v>
+        <v>1.5078075</v>
       </c>
       <c r="E29">
-        <v>1.6569593057872214</v>
+        <v>1.8847612499999999</v>
       </c>
       <c r="F29">
-        <v>1.9690497852409239</v>
+        <v>2.2617149999999997</v>
       </c>
       <c r="G29">
-        <v>2.641814432546969</v>
+        <v>3.0156225000000001</v>
       </c>
       <c r="H29">
-        <v>3.4586542687152035</v>
+        <v>3.7695299999999996</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -17689,25 +17689,25 @@
         <v>538</v>
       </c>
       <c r="B30">
-        <v>0.77589369257339103</v>
+        <v>0.90468149999999981</v>
       </c>
       <c r="C30">
-        <v>0.89199906876237101</v>
+        <v>1.13085375</v>
       </c>
       <c r="D30">
-        <v>1.3529875853259963</v>
+        <v>1.5078075</v>
       </c>
       <c r="E30">
-        <v>1.6430111636278717</v>
+        <v>1.8847612499999999</v>
       </c>
       <c r="F30">
-        <v>1.9598978914366669</v>
+        <v>2.2617149999999997</v>
       </c>
       <c r="G30">
-        <v>2.6567750002025909</v>
+        <v>3.0156225000000001</v>
       </c>
       <c r="H30">
-        <v>3.2914670522698404</v>
+        <v>3.7695299999999996</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17715,25 +17715,25 @@
         <v>539</v>
       </c>
       <c r="B31">
-        <v>0.80097686181093108</v>
+        <v>0.90468149999999981</v>
       </c>
       <c r="C31">
-        <v>0.91625118819736628</v>
+        <v>1.13085375</v>
       </c>
       <c r="D31">
-        <v>1.2645974771093185</v>
+        <v>1.5078075</v>
       </c>
       <c r="E31">
-        <v>1.6194422038895571</v>
+        <v>1.8847612499999999</v>
       </c>
       <c r="F31">
-        <v>1.9995288318498994</v>
+        <v>2.2617149999999997</v>
       </c>
       <c r="G31">
-        <v>2.7631795731251518</v>
+        <v>3.0156225000000001</v>
       </c>
       <c r="H31">
-        <v>3.3797474710500568</v>
+        <v>3.7695299999999996</v>
       </c>
     </row>
   </sheetData>
@@ -17802,14 +17802,901 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90849AF7-0A25-6F4C-8419-6629EAF8DF97}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>25</v>
+      </c>
+      <c r="D1">
+        <v>50</v>
+      </c>
+      <c r="E1">
+        <v>75</v>
+      </c>
+      <c r="F1">
+        <v>100</v>
+      </c>
+      <c r="G1">
+        <v>150</v>
+      </c>
+      <c r="H1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B2">
+        <v>0.71506606636420611</v>
+      </c>
+      <c r="C2">
+        <v>0.71875414905100699</v>
+      </c>
+      <c r="D2">
+        <v>0.71878960437917483</v>
+      </c>
+      <c r="E2">
+        <v>0.73483872890988067</v>
+      </c>
+      <c r="F2">
+        <v>0.69827372092176354</v>
+      </c>
+      <c r="G2">
+        <v>0.71132210175877486</v>
+      </c>
+      <c r="H2">
+        <v>0.71798852441300909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3">
+        <v>0.71930850747545938</v>
+      </c>
+      <c r="C3">
+        <v>0.73279883762855391</v>
+      </c>
+      <c r="D3">
+        <v>0.71950895454363284</v>
+      </c>
+      <c r="E3">
+        <v>0.67085233754564511</v>
+      </c>
+      <c r="F3">
+        <v>0.712851149029882</v>
+      </c>
+      <c r="G3">
+        <v>0.70943913644933754</v>
+      </c>
+      <c r="H3">
+        <v>0.71792916718044419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B4">
+        <v>0.72042250966937482</v>
+      </c>
+      <c r="C4">
+        <v>0.719676922381005</v>
+      </c>
+      <c r="D4">
+        <v>0.68832570326084352</v>
+      </c>
+      <c r="E4">
+        <v>0.72472727991406094</v>
+      </c>
+      <c r="F4">
+        <v>0.7178411639629052</v>
+      </c>
+      <c r="G4">
+        <v>0.72671226712123815</v>
+      </c>
+      <c r="H4">
+        <v>0.72056820032356894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B5">
+        <v>0.7327841421442034</v>
+      </c>
+      <c r="C5">
+        <v>0.75837353996422985</v>
+      </c>
+      <c r="D5">
+        <v>0.78911121476067592</v>
+      </c>
+      <c r="E5">
+        <v>0.80686308241646199</v>
+      </c>
+      <c r="F5">
+        <v>0.84193549043933091</v>
+      </c>
+      <c r="G5">
+        <v>0.96692063456835076</v>
+      </c>
+      <c r="H5">
+        <v>1.0508583090860291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B6">
+        <v>0.72886620848632955</v>
+      </c>
+      <c r="C6">
+        <v>0.7629800309157897</v>
+      </c>
+      <c r="D6">
+        <v>0.76619784691551795</v>
+      </c>
+      <c r="E6">
+        <v>0.83160345541385594</v>
+      </c>
+      <c r="F6">
+        <v>0.85258717907249248</v>
+      </c>
+      <c r="G6">
+        <v>0.95308759093767237</v>
+      </c>
+      <c r="H6">
+        <v>1.0521606268629349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B7">
+        <v>0.73249387570363367</v>
+      </c>
+      <c r="C7">
+        <v>0.77141559424394479</v>
+      </c>
+      <c r="D7">
+        <v>0.78345633332101328</v>
+      </c>
+      <c r="E7">
+        <v>0.82769712527798345</v>
+      </c>
+      <c r="F7">
+        <v>0.87717409489236253</v>
+      </c>
+      <c r="G7">
+        <v>0.93657512778600482</v>
+      </c>
+      <c r="H7">
+        <v>1.0460454927207554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B8">
+        <v>0.74545674082706359</v>
+      </c>
+      <c r="C8">
+        <v>0.77640338673542553</v>
+      </c>
+      <c r="D8">
+        <v>0.87554086006001952</v>
+      </c>
+      <c r="E8">
+        <v>0.93002386042631613</v>
+      </c>
+      <c r="F8">
+        <v>1.0135770467467382</v>
+      </c>
+      <c r="G8">
+        <v>1.1916271002672496</v>
+      </c>
+      <c r="H8">
+        <v>1.3682058128223209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>517</v>
+      </c>
+      <c r="B9">
+        <v>0.73134484996061833</v>
+      </c>
+      <c r="C9">
+        <v>0.78031584562080691</v>
+      </c>
+      <c r="D9">
+        <v>0.85344274338729187</v>
+      </c>
+      <c r="E9">
+        <v>0.9417001606580333</v>
+      </c>
+      <c r="F9">
+        <v>0.98029133960329295</v>
+      </c>
+      <c r="G9">
+        <v>1.2184403249679672</v>
+      </c>
+      <c r="H9">
+        <v>1.3883721120774239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B10">
+        <v>0.75368254108109334</v>
+      </c>
+      <c r="C10">
+        <v>0.79063935881460834</v>
+      </c>
+      <c r="D10">
+        <v>0.85136128949685708</v>
+      </c>
+      <c r="E10">
+        <v>0.95365599832833148</v>
+      </c>
+      <c r="F10">
+        <v>1.003892438666705</v>
+      </c>
+      <c r="G10">
+        <v>1.2108544348995876</v>
+      </c>
+      <c r="H10">
+        <v>1.3669423981284534</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>519</v>
+      </c>
+      <c r="B11">
+        <v>0.74151365059006102</v>
+      </c>
+      <c r="C11">
+        <v>0.78779187774599635</v>
+      </c>
+      <c r="D11">
+        <v>0.93318519185444504</v>
+      </c>
+      <c r="E11">
+        <v>0.99544307791096376</v>
+      </c>
+      <c r="F11">
+        <v>1.1515747878657849</v>
+      </c>
+      <c r="G11">
+        <v>1.3798851081578447</v>
+      </c>
+      <c r="H11">
+        <v>1.6233293932464679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>520</v>
+      </c>
+      <c r="B12">
+        <v>0.74648738640105383</v>
+      </c>
+      <c r="C12">
+        <v>0.80061919820982685</v>
+      </c>
+      <c r="D12">
+        <v>0.9228335443639154</v>
+      </c>
+      <c r="E12">
+        <v>1.0489739085129681</v>
+      </c>
+      <c r="F12">
+        <v>1.1764015544272659</v>
+      </c>
+      <c r="G12">
+        <v>1.4179965114028932</v>
+      </c>
+      <c r="H12">
+        <v>1.6201968720808102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>521</v>
+      </c>
+      <c r="B13">
+        <v>0.71791545827826397</v>
+      </c>
+      <c r="C13">
+        <v>0.78415922648608216</v>
+      </c>
+      <c r="D13">
+        <v>0.93463851901856287</v>
+      </c>
+      <c r="E13">
+        <v>0.97484918920504005</v>
+      </c>
+      <c r="F13">
+        <v>1.1376103785813734</v>
+      </c>
+      <c r="G13">
+        <v>1.409869777328929</v>
+      </c>
+      <c r="H13">
+        <v>1.6804032634972041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>522</v>
+      </c>
+      <c r="B14">
+        <v>0.74816875014755269</v>
+      </c>
+      <c r="C14">
+        <v>0.86000179250885522</v>
+      </c>
+      <c r="D14">
+        <v>0.99202876321940248</v>
+      </c>
+      <c r="E14">
+        <v>1.106882524666176</v>
+      </c>
+      <c r="F14">
+        <v>1.271525229991975</v>
+      </c>
+      <c r="G14">
+        <v>1.6630012092858513</v>
+      </c>
+      <c r="H14">
+        <v>1.9739084516002943</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B15">
+        <v>0.74402770838118248</v>
+      </c>
+      <c r="C15">
+        <v>0.83323127956731713</v>
+      </c>
+      <c r="D15">
+        <v>0.99030454057501482</v>
+      </c>
+      <c r="E15">
+        <v>1.148105671475143</v>
+      </c>
+      <c r="F15">
+        <v>1.2924488355750139</v>
+      </c>
+      <c r="G15">
+        <v>1.6286030365182178</v>
+      </c>
+      <c r="H15">
+        <v>1.9626391788486983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B16">
+        <v>0.76045102045789126</v>
+      </c>
+      <c r="C16">
+        <v>0.80575934294169627</v>
+      </c>
+      <c r="D16">
+        <v>0.99772746424023706</v>
+      </c>
+      <c r="E16">
+        <v>1.1136598290172319</v>
+      </c>
+      <c r="F16">
+        <v>1.3097505496432953</v>
+      </c>
+      <c r="G16">
+        <v>1.6368500540303836</v>
+      </c>
+      <c r="H16">
+        <v>1.9342212348138714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>525</v>
+      </c>
+      <c r="B17">
+        <v>0.75932316397975175</v>
+      </c>
+      <c r="C17">
+        <v>0.85654125388649405</v>
+      </c>
+      <c r="D17">
+        <v>1.0940566366973026</v>
+      </c>
+      <c r="E17">
+        <v>1.2641572562408654</v>
+      </c>
+      <c r="F17">
+        <v>1.3603507568514812</v>
+      </c>
+      <c r="G17">
+        <v>1.8682597554883291</v>
+      </c>
+      <c r="H17">
+        <v>2.265565520560977</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>526</v>
+      </c>
+      <c r="B18">
+        <v>0.76394055505756375</v>
+      </c>
+      <c r="C18">
+        <v>0.83955447625866475</v>
+      </c>
+      <c r="D18">
+        <v>1.077739119764803</v>
+      </c>
+      <c r="E18">
+        <v>1.2473540671058958</v>
+      </c>
+      <c r="F18">
+        <v>1.4268471575976192</v>
+      </c>
+      <c r="G18">
+        <v>1.8301032203667333</v>
+      </c>
+      <c r="H18">
+        <v>2.2374402954195487</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>527</v>
+      </c>
+      <c r="B19">
+        <v>0.76859639269493063</v>
+      </c>
+      <c r="C19">
+        <v>0.87373962763963708</v>
+      </c>
+      <c r="D19">
+        <v>1.0904070640626575</v>
+      </c>
+      <c r="E19">
+        <v>1.3009046599959579</v>
+      </c>
+      <c r="F19">
+        <v>1.3678700570538189</v>
+      </c>
+      <c r="G19">
+        <v>1.8857335756450007</v>
+      </c>
+      <c r="H19">
+        <v>2.3209693131335309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>528</v>
+      </c>
+      <c r="B20">
+        <v>0.75076441276244199</v>
+      </c>
+      <c r="C20">
+        <v>0.89181819830966214</v>
+      </c>
+      <c r="D20">
+        <v>1.0920465333961462</v>
+      </c>
+      <c r="E20">
+        <v>1.3549203941106067</v>
+      </c>
+      <c r="F20">
+        <v>1.5703040395546182</v>
+      </c>
+      <c r="G20">
+        <v>2.01710612030806</v>
+      </c>
+      <c r="H20">
+        <v>2.5935679372091425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>529</v>
+      </c>
+      <c r="B21">
+        <v>0.75215206942020041</v>
+      </c>
+      <c r="C21">
+        <v>0.91154060063879161</v>
+      </c>
+      <c r="D21">
+        <v>1.1311640039954942</v>
+      </c>
+      <c r="E21">
+        <v>1.3825586413549611</v>
+      </c>
+      <c r="F21">
+        <v>1.5084480781979113</v>
+      </c>
+      <c r="G21">
+        <v>1.995170113813534</v>
+      </c>
+      <c r="H21">
+        <v>2.5531692765459795</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>530</v>
+      </c>
+      <c r="B22">
+        <v>0.75075202637915883</v>
+      </c>
+      <c r="C22">
+        <v>0.89195921474632678</v>
+      </c>
+      <c r="D22">
+        <v>1.0701021754728139</v>
+      </c>
+      <c r="E22">
+        <v>1.2947901572792393</v>
+      </c>
+      <c r="F22">
+        <v>1.5825791590737568</v>
+      </c>
+      <c r="G22">
+        <v>2.0669666029486358</v>
+      </c>
+      <c r="H22">
+        <v>2.5658833659827831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>531</v>
+      </c>
+      <c r="B23">
+        <v>0.77808854720814047</v>
+      </c>
+      <c r="C23">
+        <v>0.97339231188897368</v>
+      </c>
+      <c r="D23">
+        <v>1.2289932118954181</v>
+      </c>
+      <c r="E23">
+        <v>1.4550010801515059</v>
+      </c>
+      <c r="F23">
+        <v>1.6462933853711921</v>
+      </c>
+      <c r="G23">
+        <v>2.268265054363432</v>
+      </c>
+      <c r="H23">
+        <v>2.8531738815834191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>532</v>
+      </c>
+      <c r="B24">
+        <v>0.75011504251102457</v>
+      </c>
+      <c r="C24">
+        <v>0.92391775522547703</v>
+      </c>
+      <c r="D24">
+        <v>1.1576837107999587</v>
+      </c>
+      <c r="E24">
+        <v>1.4384355818112371</v>
+      </c>
+      <c r="F24">
+        <v>1.6510457401620728</v>
+      </c>
+      <c r="G24">
+        <v>2.2713150393919093</v>
+      </c>
+      <c r="H24">
+        <v>2.8608978694063394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>533</v>
+      </c>
+      <c r="B25">
+        <v>0.76566754043071117</v>
+      </c>
+      <c r="C25">
+        <v>0.92281376485356748</v>
+      </c>
+      <c r="D25">
+        <v>1.2136617596610122</v>
+      </c>
+      <c r="E25">
+        <v>1.4091527486942568</v>
+      </c>
+      <c r="F25">
+        <v>1.6199667056041895</v>
+      </c>
+      <c r="G25">
+        <v>2.3223452272518079</v>
+      </c>
+      <c r="H25">
+        <v>2.7962117981393888</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>534</v>
+      </c>
+      <c r="B26">
+        <v>0.71100664638581534</v>
+      </c>
+      <c r="C26">
+        <v>1.0160446101234422</v>
+      </c>
+      <c r="D26">
+        <v>1.2223302609742199</v>
+      </c>
+      <c r="E26">
+        <v>1.5737299995929364</v>
+      </c>
+      <c r="F26">
+        <v>1.8140642925867696</v>
+      </c>
+      <c r="G26">
+        <v>2.4965088734340215</v>
+      </c>
+      <c r="H26">
+        <v>3.1705133391543554</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>535</v>
+      </c>
+      <c r="B27">
+        <v>0.772714033380697</v>
+      </c>
+      <c r="C27">
+        <v>0.8926641220591025</v>
+      </c>
+      <c r="D27">
+        <v>1.2223601351633306</v>
+      </c>
+      <c r="E27">
+        <v>1.5389342867585005</v>
+      </c>
+      <c r="F27">
+        <v>1.7969707715812695</v>
+      </c>
+      <c r="G27">
+        <v>2.5207792896816907</v>
+      </c>
+      <c r="H27">
+        <v>3.2370190613221776</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>536</v>
+      </c>
+      <c r="B28">
+        <v>0.77669151330420372</v>
+      </c>
+      <c r="C28">
+        <v>0.94544055628202328</v>
+      </c>
+      <c r="D28">
+        <v>1.2976233116485889</v>
+      </c>
+      <c r="E28">
+        <v>1.5756365434182478</v>
+      </c>
+      <c r="F28">
+        <v>1.8075258575785609</v>
+      </c>
+      <c r="G28">
+        <v>2.4602937099866953</v>
+      </c>
+      <c r="H28">
+        <v>3.1584168705730828</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>537</v>
+      </c>
+      <c r="B29">
+        <v>0.7804707471730471</v>
+      </c>
+      <c r="C29">
+        <v>0.9776623785413846</v>
+      </c>
+      <c r="D29">
+        <v>1.3761953177319712</v>
+      </c>
+      <c r="E29">
+        <v>1.6569593057872214</v>
+      </c>
+      <c r="F29">
+        <v>1.9690497852409239</v>
+      </c>
+      <c r="G29">
+        <v>2.641814432546969</v>
+      </c>
+      <c r="H29">
+        <v>3.4586542687152035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>538</v>
+      </c>
+      <c r="B30">
+        <v>0.77589369257339103</v>
+      </c>
+      <c r="C30">
+        <v>0.89199906876237101</v>
+      </c>
+      <c r="D30">
+        <v>1.3529875853259963</v>
+      </c>
+      <c r="E30">
+        <v>1.6430111636278717</v>
+      </c>
+      <c r="F30">
+        <v>1.9598978914366669</v>
+      </c>
+      <c r="G30">
+        <v>2.6567750002025909</v>
+      </c>
+      <c r="H30">
+        <v>3.2914670522698404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B31">
+        <v>0.80097686181093108</v>
+      </c>
+      <c r="C31">
+        <v>0.91625118819736628</v>
+      </c>
+      <c r="D31">
+        <v>1.2645974771093185</v>
+      </c>
+      <c r="E31">
+        <v>1.6194422038895571</v>
+      </c>
+      <c r="F31">
+        <v>1.9995288318498994</v>
+      </c>
+      <c r="G31">
+        <v>2.7631795731251518</v>
+      </c>
+      <c r="H31">
+        <v>3.3797474710500568</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D31">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B31">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:H32">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:H31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E28CD23-4C6F-DF4A-A8B2-BAE2FA4DD71E}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">

</xml_diff>